<commit_message>
Solver.py ve order_planner.py güncellendi
</commit_message>
<xml_diff>
--- a/pyhton kodlar.xlsx
+++ b/pyhton kodlar.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\trkizilkbu\Order_Planner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3066592F-E60C-45B2-A018-DE765EC299AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8F1FECE7-93F8-44C4-BA71-B3D6E988F7FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{3FCAF020-D2FD-40E6-A1F3-D81AA00CDAE1}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{3FCAF020-D2FD-40E6-A1F3-D81AA00CDAE1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
   <si>
     <t>solver.py</t>
   </si>
@@ -252,60 +252,237 @@
         </t>
   </si>
   <si>
-    <t>import pandas as pd
+    <t>Kullanılan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">import streamlit as st
+import pandas as pd
+from solver import solve_assignment
+from io import BytesIO
+from PIL import Image
+# CSS ile yazı tipi ve boyutu ayarlayalım
+st.markdown("""
+    &lt;style&gt;
+        div[data-testid="stDataFrame"] div[role="gridcell"] {
+            font-family: Calibri, sans-serif;
+            font-size: 9pt;
+        }
+        .dataframe {
+            font-family: Calibri, sans-serif;
+            font-size: 9pt;
+        }
+    &lt;/style&gt;
+""", unsafe_allow_html=True)
+# Sayfanın başına ortalanmış resim ekle
+image = Image.open("Picture1.png")
+st.markdown("&lt;div style='text-align: center;'&gt;", unsafe_allow_html=True)
+st.image(image, width=300)
+st.markdown("&lt;/div&gt;", unsafe_allow_html=True)
+st.title("🚛 Load Planner")
+uploaded_file = st.file_uploader("Sipariş dosyasını yükleyin (Excel)", type=["xlsx"])
+if uploaded_file:
+    order_df = pd.read_excel(uploaded_file)
+    st.subheader("📝Yüklenen Sipariş Verisi")
+    st.dataframe(order_df, use_container_width=True, height=400)
+        # Bilgi Kartları Bölümü - Dosya yüklenince hemen çalışır
+    st.subheader("🔍 Veri Kalite Kontrolleri")
+    total_orders = order_df['Sales Document'].nunique()
+    missing_paltype = order_df[order_df['PALTypeChoice'].isna()]
+    missing_city = order_df[order_df['City_District'].isna()]
+    # Renk belirleme
+    paltype_color = "#90ee90" if missing_paltype.empty else "#ff7f7f"
+    city_color = "#90ee90" if missing_city.empty else "#ff7f7f"
+    col1, col2, col3 = st.columns(3)
+    with col1:
+        st.markdown(f"""
+            &lt;div style='padding: 20px; background-color: #90ee90; border-radius: 10px; text-align: center'&gt;
+                &lt;h4 style='margin: 0'&gt;Planda {total_orders} sipariş var&lt;/h4&gt;
+            &lt;/div&gt;
+        """, unsafe_allow_html=True)
+    with col2:
+        st.markdown(f"""
+            &lt;div style='padding: 20px; background-color: {paltype_color}; border-radius: 10px; text-align: center'&gt;
+                &lt;h4 style='margin: 0'&gt;
+                    {len(missing_paltype)} adet siparişin 'PALTypeChoice' bilgisi eksik.&lt;br&gt;Kontrol edin.
+                &lt;/h4&gt;
+            &lt;/div&gt;
+        """, unsafe_allow_html=True)
+    with col3:
+        st.markdown(f"""
+            &lt;div style='padding: 20px; background-color: {city_color}; border-radius: 10px; text-align: center'&gt;
+                &lt;h4 style='margin: 0'&gt;
+                    {missing_city['Ship to'].nunique()} adet müşterinin 'City_District' bilgisi eksik.&lt;br&gt;Kontrol edin.
+                &lt;/h4&gt;
+            &lt;/div&gt;
+        """, unsafe_allow_html=True)
+    if st.button("Araca Atamaları Yap"):
+        assigned_df = solve_assignment(order_df)
+        st.subheader("🚚 Atama Sonuçları")
+        st.dataframe(assigned_df, use_container_width=True, height=500)
+        # Araç bazlı özet tablo
+        summary = assigned_df.groupby("Assigned_Truck").agg({
+            'CPallet': 'sum',
+            'CPallet_M3': 'sum',
+            'CPallet_Gross': 'sum',
+            'EffectivePallet': 'sum'
+        }).reset_index()
+        # Doluluk hesaplaması: kamyon mu tır mı kontrol et
+        def hesapla_doluluk_satiri(row):
+            if row['EffectivePallet'] &lt;= 18:
+                palet_kapasite = 18
+                hacim_kapasite = 44
+                agirlik_kapasite = 12000
+            else:
+                palet_kapasite = 33
+                hacim_kapasite = 82
+                agirlik_kapasite = 24000
+            return pd.Series({
+                'DolulukOrani_Pallet': (row['EffectivePallet'] / palet_kapasite) * 100,
+                'DolulukOrani_Volume': (row['CPallet_M3'] / hacim_kapasite) * 100,
+                'DolulukOrani_Weight': (row['CPallet_Gross'] / agirlik_kapasite) * 100
+            })
+        doluluk_df = summary.apply(hesapla_doluluk_satiri, axis=1)
+        summary = pd.concat([summary, doluluk_df], axis=1)
+        def renk_kodla(deger):
+            if deger &gt;= 95:
+                return 'background-color: lightgreen'
+            elif deger &gt;= 70:
+                return 'background-color: yellow'
+            else:
+                return 'background-color: lightcoral'
+        st.subheader("📊Araç Bazlı Özet")
+        styled_summary = summary.style \
+            .applymap(renk_kodla, subset=['DolulukOrani_Pallet']) \
+            .format({
+                'DolulukOrani_Pallet': "{:.1f}%",
+                'DolulukOrani_Volume': "{:.1f}%",
+                'DolulukOrani_Weight': "{:.1f}%"
+            })
+        st.dataframe(styled_summary, use_container_width=True, height=500)
+        # Yeni detaylı özet tablo (Araç + Ship-to bazlı)
+        truck_shipto_summary = assigned_df.groupby(
+            ['Assigned_Truck', 'Ship to', 'Ship to name', 'City_District','Sales Document','Requested delivery d']
+        )['EffectivePallet'].sum().reset_index()
+        st.subheader("Araç &amp; Ship-to Detaylı Özet")
+        st.dataframe(truck_shipto_summary, use_container_width=True, height=400)
+        # Excel çıktısı
+        output = BytesIO()
+        with pd.ExcelWriter(output, engine='xlsxwriter') as writer:
+            assigned_df.to_excel(writer, index=False, sheet_name='Atama Sonuçları')
+            summary.to_excel(writer, index=False, sheet_name='Araç Özeti')
+            truck_shipto_summary.to_excel(writer, index=False, sheet_name='Araç-ShipTo Özeti')
+        output.seek(0)
+        st.download_button(
+            label="📥 Excel İndir (Atama + Özetler)",
+            data=output,
+            file_name="order_arac_atama.xlsx",
+            mime="application/vnd.openxmlformats-officedocument.spreadsheetml.sheet"
+        )
+        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">import pandas as pd
 def palet_factor(pal_type):
     return 0.5 if pal_type == 'Kısa Hafif' else 1
 def calculate_effective_pallet(row):
     return row['CPallet'] * palet_factor(row['PALTypeChoice'])
-def split_row_proportionally(row, split_factor):
-    new_row = row.copy()
-    for col in ['Order_Confirmed_Quan', 'CPallet', 'EffectivePallet']:
-        if col in row:
-            new_row[col] = row[col] * split_factor
-    return new_row
-def assign_orders_to_trucks(order_rows, truck_counter, assignments, max_pallet_limit, truck_type_name):
-    """
-    Verilen siparişleri sırayla araca at, max_pallet_limit kadar toplam palet kabul et.
-    """
-    pending_rows = order_rows.copy()
-    while pending_rows:
-        current_load = 0.0
-        current_truck_orders = []
-        remaining_rows = []
-        for row in pending_rows:
-            ep = row['EffectivePallet']
-            if current_load + ep &lt;= max_pallet_limit:
-                current_truck_orders.append(row)
-                current_load += ep
-            else:
-                remaining_capacity = max_pallet_limit - current_load
-                if remaining_capacity &gt; 0:
-                    # Satırı böl, kalan kapasiteyi doldur
-                    split_factor = remaining_capacity / ep
-                    partial_row = split_row_proportionally(row, split_factor)
-                    current_truck_orders.append(partial_row)
-                    current_load += partial_row['EffectivePallet']
-                    remaining_factor = 1 - split_factor
-                    remaining_row = split_row_proportionally(row, remaining_factor)
-                    remaining_rows.append(remaining_row)
+def split_large_orders(city_group, truck_counter_start=1):
+    """33 paleti geçen büyük siparişleri böl ve 33 paletlik parçaları ata,
+    kalanları da liste olarak döndür."""
+    assignments = []
+    leftover_parts = []
+    truck_counter = truck_counter_start
+    shipto_groups = city_group.groupby('Ship to')
+    for ship_to, sub_group in shipto_groups:
+        total_pallet = sub_group['EffectivePallet'].sum()
+        if total_pallet &lt;= 33:
+            # Küçük siparişler burada değil, sonraya bırakacağız
+            leftover_parts.append((ship_to, sub_group))
+            continue
+        # Büyük siparişleri böl
+        rows = sub_group.to_dict('records')
+        part = []
+        part_load = 0
+        for row in rows:
+            p = row['EffectivePallet']
+            if part_load + p &gt; 33:
+                # 33 paleti geçen parça tamamlanınca ata
+                df_part = pd.DataFrame(part)
+                for r in df_part.to_dict('records'):
+                    r['Assigned_Truck'] = f"Truck-{truck_counter}"
+                    assignments.append(r)
+                truck_counter += 1
+                part = []
+                part_load = 0
+            part.append(row)
+            part_load += p
+        # Kalan parçayı atama listesine ekle
+        if part:
+            df_part = pd.DataFrame(part)
+            leftover_parts.append((ship_to, df_part))
+    return assignments, leftover_parts, truck_counter
+def group_and_assign_leftovers(leftover_parts, truck_counter_start=1):
+    """Kalan parçaları şehir bazında grupla, 33 palet ve 4 shipto kısıtları ile araçlara ata."""
+    assignments = []
+    truck_counter = truck_counter_start
+    # leftover_parts: list of (ship_to, DataFrame)
+    # Önce ship_to bazında grupla ve tüm DataFrame'leri birleştir
+    combined_df = pd.concat([df for _, df in leftover_parts], ignore_index=True)
+    # Şehir bazında grupla
+    grouped_city = combined_df.groupby('Ship to City')
+    for city, city_group in grouped_city:
+        city_group = city_group.reset_index(drop=True)
+        # Ship to bazında grupla
+        subgroups = city_group.groupby('Ship to')
+        pending_groups = []
+        for ship_to, sub_group in subgroups:
+            total_pallet = sub_group['EffectivePallet'].sum()
+            pending_groups.append((ship_to, sub_group, total_pallet))
+        # Palet sayısına göre azalan sırala
+        pending_groups.sort(key=lambda x: x[2], reverse=True)
+        while pending_groups:
+            current_load = 0
+            truck_orders = []
+            used_shiptos = set()
+            remaining_groups = []
+            def calc_adjusted_pallet(sub_group, multiple_shipto):
+                if not multiple_shipto:
+                    return sub_group['EffectivePallet'].sum()
                 else:
-                    remaining_rows.append(row)
-        for r in current_truck_orders:
-            r['Assigned_Truck'] = f"Truck-{truck_counter} - {truck_type_name}"
-            assignments.append(r)
-        print(f"🚚 Truck-{truck_counter} - {truck_type_name} =&gt; {len(current_truck_orders)} kayıt | {current_load:.2f} Effective Pallet")
-        truck_counter += 1
-        pending_rows = remaining_rows
-    return truck_counter
+                    def pallet_factor_override(row):
+                        if row['PALTypeChoice'] == 'Kısa Hafif':
+                            return row['CPallet'] * 1
+                        else:
+                            return row['CPallet'] * 1
+                    return sub_group.apply(pallet_factor_override, axis=1).sum()
+            for ship_to, sub_group, total_pallet in pending_groups:
+                multiple_shipto_in_truck = len(used_shiptos | {ship_to}) &gt; 1
+                adjusted_pallet = calc_adjusted_pallet(sub_group, multiple_shipto_in_truck)
+                if adjusted_pallet &lt;= 33:
+                    if (current_load + adjusted_pallet &lt;= 33) and (len(used_shiptos | {ship_to}) &lt;= 4):
+                        current_load += adjusted_pallet
+                        truck_orders.append((ship_to, sub_group))
+                        used_shiptos.add(ship_to)
+                    else:
+                        remaining_groups.append((ship_to, sub_group, total_pallet))
+                else:
+                    remaining_groups.append((ship_to, sub_group, total_pallet))
+            if truck_orders:
+                for ship_to, sub_group in truck_orders:
+                    for _, row in sub_group.iterrows():
+                        order = row.to_dict()
+                        order['Assigned_Truck'] = f"Truck-{truck_counter}"
+                        assignments.append(order)
+                truck_counter += 1
+            pending_groups = remaining_groups
+    return assignments, truck_counter
 def solve_assignment(order_df):
     order_df = order_df.copy()
     order_df.columns = order_df.columns.str.strip()
     order_df = order_df.reset_index(drop=True)
-    required_cols = ['Ship to City', 'Ship to', 'Truck_Type', 'Ship to name', 'PALTypeChoice', 'CPallet']
-    for col in required_cols:
-        if col not in order_df.columns:
-            print(f"HATA: Gerekli sütun eksik: {col}")
-            return pd.DataFrame()
+    if 'Ship to City' not in order_df.columns or 'Ship to' not in order_df.columns:
+        print("HATA: Gerekli sütunlar eksik!")
+        return pd.DataFrame()
     try:
         order_df['EffectivePallet'] = order_df.apply(calculate_effective_pallet, axis=1)
     except Exception as e:
@@ -313,257 +490,37 @@
         return pd.DataFrame()
     assignments = []
     truck_counter = 1
-    # 🎯 Öncelikli müşteri kontrolü: Ozdilek + Bursa
-    ozdilek_mask = (
-        (order_df['Ship to name'].str.strip().str.lower() == 'ozdilek alisveris merkezleri') &amp;
-        (order_df['Ship to City'].str.strip().str.lower() == 'bursa')
-    )
-    ozdilek_df = order_df[ozdilek_mask].copy()
-    remaining_df = order_df[~ozdilek_mask].copy()
-    if not ozdilek_df.empty:
-        print("\n🎯 Özel grup: Ozdilek Alisveris Merkezleri - Bursa işleniyor...")
-        ozdilek_rows = [r.to_dict() for _, r in ozdilek_df.iterrows()]
-        ozdilek_rows.sort(key=lambda x: x['EffectivePallet'], reverse=True)
-        truck_counter = assign_orders_to_trucks(ozdilek_rows, truck_counter, assignments, 33, "Tır")
-    # 🚛 Aşama 1: Kamyon siparişlerini şehir bazında grupla
-    kamyon_df = remaining_df[remaining_df['Truck_Type'] == 'Kamyon'].copy()
-    tir_df = remaining_df[remaining_df['Truck_Type'] == 'Tır'].copy()
-    other_df = remaining_df[~remaining_df['Truck_Type'].isin(['Kamyon', 'Tır'])].copy()
-    grouped_city = kamyon_df.groupby('Ship to City')
-    kamyon_assigned_indices = set()
-    tir_assigned_indices = set()
-    # Her şehir için kamyon siparişlerini at
+    grouped_city = order_df.groupby('Ship to City')
     for city, city_group in grouped_city:
-        city_kamyon_orders = city_group.sort_values(by='EffectivePallet', ascending=False).to_dict('records')
-        # Kamyon siparişleriyle araçlar oluştur
-        pending_kamyon_orders = city_kamyon_orders.copy()
-        while pending_kamyon_orders:
-            current_load = 0.0
-            current_truck_orders = []
-            remaining_kamyon = []
-            # Kamyon siparişlerini doldur
-            for row in pending_kamyon_orders:
-                ep = row['EffectivePallet']
-                if current_load + ep &lt;= 18:
-                    current_truck_orders.append(row)
-                    current_load += ep
-                else:
-                    remaining_capacity = 18 - current_load
-                    if remaining_capacity &gt; 0:
-                        split_factor = remaining_capacity / ep
-                        partial_row = split_row_proportionally(row, split_factor)
-                        current_truck_orders.append(partial_row)
-                        current_load += partial_row['EffectivePallet']
-                        remaining_factor = 1 - split_factor
-                        remaining_row = split_row_proportionally(row, remaining_factor)
-                        remaining_kamyon.append(remaining_row)
-                    else:
-                        remaining_kamyon.append(row)
-            # Kamyon siparişleri dolduruldu, şimdi tır siparişlerinden ekleme yap
-            city_tir_orders = tir_df[tir_df['Ship to City'] == city].sort_values(by='EffectivePallet', ascending=False).to_dict('records')
-            pending_tir_orders = city_tir_orders.copy()
-            remaining_tir = []
-            for row in pending_tir_orders:
-                ep = row['EffectivePallet']
-                if current_load + ep &lt;= 18:
-                    current_truck_orders.append(row)
-                    current_load += ep
-                    tir_assigned_indices.add(row['index'] if 'index' in row else None)
-                else:
-                    remaining_capacity = 18 - current_load
-                    if remaining_capacity &gt; 0:
-                        split_factor = remaining_capacity / ep
-                        partial_row = split_row_proportionally(row, split_factor)
-                        current_truck_orders.append(partial_row)
-                        current_load += partial_row['EffectivePallet']
-                        remaining_factor = 1 - split_factor
-                        remaining_row = split_row_proportionally(row, remaining_factor)
-                        remaining_tir.append(remaining_row)
-                    else:
-                        remaining_tir.append(row)
-            # Atama yap
-            for r in current_truck_orders:
-                r['Assigned_Truck'] = f"Truck-{truck_counter} - Kamyon"
-                assignments.append(r)
-            print(f"🚚 Truck-{truck_counter} - Kamyon =&gt; {len(current_truck_orders)} kayıt | {current_load:.2f} Effective Pallet | Şehir: {city}")
-            truck_counter += 1
-            pending_kamyon_orders = remaining_kamyon
-            tir_df = tir_df[~tir_df.index.isin(tir_assigned_indices)]
-    # Geriye kalan tır siparişlerini şehir bazında 33 palet limiti ile ata
-    grouped_city_tir = tir_df.groupby('Ship to City')
-    for city, city_group in grouped_city_tir:
-        city_tir_orders = city_group.sort_values(by='EffectivePallet', ascending=False).to_dict('records')
-        truck_counter = assign_orders_to_trucks(city_tir_orders, truck_counter, assignments, 33, "Tır")
-    # Diğer tip siparişleri 33 palet limiti ile ata (şehir bazında)
-    grouped_city_other = other_df.groupby('Ship to City')
-    for city, city_group in grouped_city_other:
-        city_orders = city_group.sort_values(by='EffectivePallet', ascending=False).to_dict('records')
-        truck_counter = assign_orders_to_trucks(city_orders, truck_counter, assignments, 33, "Diğer")
-    print(f"\n✅ Toplam atanan kayıt: {len(assignments)}")
-    return pd.DataFrame(assignments)</t>
-  </si>
-  <si>
-    <t>Kullanılan</t>
-  </si>
-  <si>
-    <t>İl Kombinasyonlu</t>
-  </si>
-  <si>
-    <t>İl Kombinasyonuz-Kamyon</t>
-  </si>
-  <si>
-    <t>import pandas as pd
-# ————————————————————————————————————————————————————————————————————
-# Yardımcı fonksiyonlar
-# ————————————————————————————————————————————————————————————————————
-def palet_factor(pal_type: str) -&gt; float:
-    """Palet tipine göre katsayı döndür."""
-    return 0.5 if pal_type == "Kısa Hafif" else 1.0
-def calculate_effective_pallet(row: pd.Series) -&gt; float:
-    """Satır bazlı efektif palet değeri."""
-    return row["CPallet"] * palet_factor(row["PALTypeChoice"])
-def get_truck_type(pallet_sum: float) -&gt; str:
-    """
-    Palet toplamına göre aracın gövde tipini döndür.
-    ≤ 18  → Kamyon
-    ≥ 19  → Tır
-    """
-    return "Kamyon" if pallet_sum &lt;= 18 else "Tır"
-def get_temp_prefix(df: pd.DataFrame) -&gt; str:
-    """
-    Temp_Type sütununa göre araç için sıcaklık ön ekini döndür.
-    - En az bir “Temp” varsa  → Frigo
-    - Aksi hâlde (tamamı Ambient) → Tente
-    Sütun yoksa da “Tente” varsayılır.
-    """
-    if "Temp_Type" not in df.columns:
-        return "Tente"
-    is_temp = (
-        df["Temp_Type"]
-        .astype(str)
-        .str.strip()
-        .str.lower()
-        .eq("temp")
-        .any()
-    )
-    return "Frigo" if is_temp else "Tente"
-# ————————————————————————————————————————————————————————————————————
-# Ana çözümleyici
-# ————————————————————————————————————————————————————————————————————
-def solve_assignment(order_df: pd.DataFrame) -&gt; pd.DataFrame:
-    """
-    Parametre: order_df – sipariş verisi
-    Dönüş   : ataması yapılmış sipariş satırlarını içeren DataFrame
-    """
-    order_df = order_df.copy()
-    order_df.columns = order_df.columns.str.strip()
-    order_df = order_df.reset_index(drop=True)
-    if "Ship to City" not in order_df.columns or "Ship to" not in order_df.columns:
-        print("HATA: Gerekli sütunlar eksik!")
-        return pd.DataFrame()
-    # Efektif palet hesabı
-    try:
-        order_df["EffectivePallet"] = order_df.apply(calculate_effective_pallet, axis=1)
-    except Exception as e:
-        print("EffectivePallet hesaplamasında hata:", e)
-        return pd.DataFrame()
-    assignments = []
-    truck_counter = 1
-    # Şehir kombinasyonları
-    city_combinations = [
-        {"Bursa", "Yalova"},
-        {"Balikesir", "Canakkale"},
-        {"Mugla", "Aydin"},
-    ]
-    leftover_groups = []  # Küçük / orta yükler burada tutulur
-    # ——— 1) Şehir bazlı ön atama ——————————————————————————————
-    grouped_city = order_df.groupby("Ship to City")
-    for city, city_group in grouped_city:
-        print(f"\n🛻 Atama işlemi başlatıldı – {city} ({len(city_group)} kayıt)")
-        city_group = city_group.reset_index(drop=True)
-        subgroups = city_group.groupby("Ship to")
-        for ship_to, sub_group in subgroups:
-            total_pallet = sub_group["EffectivePallet"].sum()
-            print(f"  ▶ Ship-to: {ship_to} | Toplam Palet: {total_pallet:.2f}")
-            if total_pallet &gt; 33:
-                # Büyük grup → doğrudan atama
-                truck_type = get_truck_type(total_pallet)
-                temp_prefix = get_temp_prefix(sub_group)
-                truck_name = f"{temp_prefix} {truck_type}-{truck_counter}"
-                for _, row in sub_group.iterrows():
-                    order = row.to_dict()
-                    order["Assigned_Truck"] = truck_name
-                    assignments.append(order)
-                print(
-                    f"🚚 {truck_name} ⇒ Ship-to {ship_to} "
-                    f"(büyük grup) | {total_pallet:.2f} Palet"
-                )
-                truck_counter += 1
-            else:
-                # Küçük / orta yükler daha sonra birleştirilecek
-                leftover_groups.append((city, ship_to, sub_group, total_pallet))
-    # ——— 2) Küçük yükleri şehir kombinasyonlarına göre birleştir ———
-    normalize = lambda c: c.strip().lower()
-    city_group_map = {}
-    for city, ship_to, sub_group, total_pallet in leftover_groups:
-        city_norm = normalize(city)
-        city_group_map.setdefault(city_norm, []).append(
-            (ship_to, sub_group, total_pallet)
-        )
-    normalized_combinations = [set(map(normalize, comb)) for comb in city_combinations]
-    city_comb_group_map = {}
-    for city_norm, groups in city_group_map.items():
-        placed = False
-        for comb in normalized_combinations:
-            if city_norm in comb:
-                city_comb_group_map.setdefault(frozenset(comb), []).extend(groups)
-                placed = True
-                break
-        if not placed:
-            city_comb_group_map.setdefault(frozenset({city_norm}), []).extend(groups)
-    # ——— Kombinasyon bazlı atama ——————————————————————————————
-    for comb_key, group_list in city_comb_group_map.items():
-        comb_cities = list(comb_key)
-        print(f"\n🔗 Kombinasyon ile atama: {comb_cities} ({len(group_list)} grup)")
-        group_list.sort(key=lambda x: x[2], reverse=True)  # büyükten küçüğe
-        pending_groups = group_list.copy()
-        while pending_groups:
-            current_load = 0.0
-            truck_orders = []
-            used_shiptos = set()
-            remaining = []
-            for ship_to, sub_group, total_pallet in pending_groups:
-                if (
-                    total_pallet &lt;= 33
-                    and current_load + total_pallet &lt;= 33
-                    and len(used_shiptos | {ship_to}) &lt;= 4
-                ):
-                    current_load += total_pallet
-                    truck_orders.append((ship_to, sub_group))
-                    used_shiptos.add(ship_to)
-                else:
-                    remaining.append((ship_to, sub_group, total_pallet))
-            if truck_orders:
-                # Tek seferde bu araca atanacak tüm grupları birleştir
-                df_truck = pd.concat([sg for _, sg in truck_orders], ignore_index=True)
-                truck_type = get_truck_type(current_load)
-                temp_prefix = get_temp_prefix(df_truck)
-                truck_name = f"{temp_prefix} {truck_type}-{truck_counter}"
-                for _, sub_group in truck_orders:
-                    for _, row in sub_group.iterrows():
-                        order = row.to_dict()
-                        order["Assigned_Truck"] = truck_name
-                        assignments.append(order)
-                print(
-                    f"🚚 {truck_name} ⇒ Kombinasyon ataması "
-                    f"| Toplam Palet: {current_load:.2f}"
-                )
-                truck_counter += 1
-            else:
-                break  # Daha fazla gruplanamıyor
-            pending_groups = remaining
-    print(f"\n✅ Toplam atanan kayıt: {len(assignments)}")
-    return pd.DataFrame(assignments)</t>
+        # 1. Büyük siparişleri böl ve 33 paletlik parçaları ata
+        assigned_large, leftover_parts, truck_counter = split_large_orders(city_group, truck_counter)
+        assignments.extend(assigned_large)
+        # 2. Kalan parçalarla şehir bazında gruplayarak araçlara ata
+        assigned_leftovers, truck_counter = group_and_assign_leftovers(leftover_parts, truck_counter)
+        assignments.extend(assigned_leftovers)
+    # assignments listesini DataFrame'e çevir
+    assigned_df = pd.DataFrame(assignments)
+    # Burada Assigned_Truck bazında araç isimlerini güncelleyelim
+    def update_truck_name(truck_id, df):
+        # Araçta Temp_Type sütununda 'Temp' geçen var mı kontrolü
+        has_temp = df['Temp_Type'].astype(str).str.contains('Temp').any()
+        truck_type = "Frigo" if has_temp else "Tente"
+        total_pallet = df['EffectivePallet'].sum()
+        vehicle_type = "Kamyon" if total_pallet &lt;= 18 else "Tır"
+        return f"{truck_type} {vehicle_type} -{truck_id}"
+    # Assigned_Truck sütunundaki değerlerden sadece sayıyı alalım (örneğin 'Truck-3' -&gt; 3)
+    assigned_df['Truck_Number'] = assigned_df['Assigned_Truck'].str.extract(r'(\d+)').astype(int)
+    # Araç bazında yeni isimler oluştur
+    truck_names = {}
+    for truck_num, group in assigned_df.groupby('Truck_Number'):
+        truck_names[truck_num] = update_truck_name(truck_num, group)
+    # Yeni isimleri Assigned_Truck sütununa yaz
+    assigned_df['Assigned_Truck'] = assigned_df['Truck_Number'].map(truck_names)
+    # Yardımcı sütunu kaldıralım
+    assigned_df = assigned_df.drop(columns=['Truck_Number'])
+    print(f"\n✅ Toplam atanan kayıt: {len(assigned_df)}")
+    return assigned_df
+</t>
   </si>
 </sst>
 </file>
@@ -640,7 +597,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -652,10 +609,9 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1000,26 +956,26 @@
   <cols>
     <col min="1" max="1" width="16.81640625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.453125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="29.90625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="22.6328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.453125" style="1" customWidth="1"/>
     <col min="5" max="16384" width="16.7265625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>7</v>
+        <v>4</v>
+      </c>
+      <c r="C1" s="5">
+        <v>45821</v>
+      </c>
+      <c r="D1" s="5">
+        <v>45821</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="18.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1030,7 +986,7 @@
         <v>0</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
@@ -1041,10 +997,10 @@
         <v>3</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improve split logic: sales document based assignment; enhanced splitting for oversized docs; update requirements
</commit_message>
<xml_diff>
--- a/pyhton kodlar.xlsx
+++ b/pyhton kodlar.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\trkizilkbu\Order_Planner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8F1FECE7-93F8-44C4-BA71-B3D6E988F7FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4EB5B34-E6C3-4ACA-A4A4-53F645751CE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{3FCAF020-D2FD-40E6-A1F3-D81AA00CDAE1}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{3FCAF020-D2FD-40E6-A1F3-D81AA00CDAE1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="13">
   <si>
     <t>solver.py</t>
   </si>
@@ -255,132 +255,6 @@
     <t>Kullanılan</t>
   </si>
   <si>
-    <t xml:space="preserve">import streamlit as st
-import pandas as pd
-from solver import solve_assignment
-from io import BytesIO
-from PIL import Image
-# CSS ile yazı tipi ve boyutu ayarlayalım
-st.markdown("""
-    &lt;style&gt;
-        div[data-testid="stDataFrame"] div[role="gridcell"] {
-            font-family: Calibri, sans-serif;
-            font-size: 9pt;
-        }
-        .dataframe {
-            font-family: Calibri, sans-serif;
-            font-size: 9pt;
-        }
-    &lt;/style&gt;
-""", unsafe_allow_html=True)
-# Sayfanın başına ortalanmış resim ekle
-image = Image.open("Picture1.png")
-st.markdown("&lt;div style='text-align: center;'&gt;", unsafe_allow_html=True)
-st.image(image, width=300)
-st.markdown("&lt;/div&gt;", unsafe_allow_html=True)
-st.title("🚛 Load Planner")
-uploaded_file = st.file_uploader("Sipariş dosyasını yükleyin (Excel)", type=["xlsx"])
-if uploaded_file:
-    order_df = pd.read_excel(uploaded_file)
-    st.subheader("📝Yüklenen Sipariş Verisi")
-    st.dataframe(order_df, use_container_width=True, height=400)
-        # Bilgi Kartları Bölümü - Dosya yüklenince hemen çalışır
-    st.subheader("🔍 Veri Kalite Kontrolleri")
-    total_orders = order_df['Sales Document'].nunique()
-    missing_paltype = order_df[order_df['PALTypeChoice'].isna()]
-    missing_city = order_df[order_df['City_District'].isna()]
-    # Renk belirleme
-    paltype_color = "#90ee90" if missing_paltype.empty else "#ff7f7f"
-    city_color = "#90ee90" if missing_city.empty else "#ff7f7f"
-    col1, col2, col3 = st.columns(3)
-    with col1:
-        st.markdown(f"""
-            &lt;div style='padding: 20px; background-color: #90ee90; border-radius: 10px; text-align: center'&gt;
-                &lt;h4 style='margin: 0'&gt;Planda {total_orders} sipariş var&lt;/h4&gt;
-            &lt;/div&gt;
-        """, unsafe_allow_html=True)
-    with col2:
-        st.markdown(f"""
-            &lt;div style='padding: 20px; background-color: {paltype_color}; border-radius: 10px; text-align: center'&gt;
-                &lt;h4 style='margin: 0'&gt;
-                    {len(missing_paltype)} adet siparişin 'PALTypeChoice' bilgisi eksik.&lt;br&gt;Kontrol edin.
-                &lt;/h4&gt;
-            &lt;/div&gt;
-        """, unsafe_allow_html=True)
-    with col3:
-        st.markdown(f"""
-            &lt;div style='padding: 20px; background-color: {city_color}; border-radius: 10px; text-align: center'&gt;
-                &lt;h4 style='margin: 0'&gt;
-                    {missing_city['Ship to'].nunique()} adet müşterinin 'City_District' bilgisi eksik.&lt;br&gt;Kontrol edin.
-                &lt;/h4&gt;
-            &lt;/div&gt;
-        """, unsafe_allow_html=True)
-    if st.button("Araca Atamaları Yap"):
-        assigned_df = solve_assignment(order_df)
-        st.subheader("🚚 Atama Sonuçları")
-        st.dataframe(assigned_df, use_container_width=True, height=500)
-        # Araç bazlı özet tablo
-        summary = assigned_df.groupby("Assigned_Truck").agg({
-            'CPallet': 'sum',
-            'CPallet_M3': 'sum',
-            'CPallet_Gross': 'sum',
-            'EffectivePallet': 'sum'
-        }).reset_index()
-        # Doluluk hesaplaması: kamyon mu tır mı kontrol et
-        def hesapla_doluluk_satiri(row):
-            if row['EffectivePallet'] &lt;= 18:
-                palet_kapasite = 18
-                hacim_kapasite = 44
-                agirlik_kapasite = 12000
-            else:
-                palet_kapasite = 33
-                hacim_kapasite = 82
-                agirlik_kapasite = 24000
-            return pd.Series({
-                'DolulukOrani_Pallet': (row['EffectivePallet'] / palet_kapasite) * 100,
-                'DolulukOrani_Volume': (row['CPallet_M3'] / hacim_kapasite) * 100,
-                'DolulukOrani_Weight': (row['CPallet_Gross'] / agirlik_kapasite) * 100
-            })
-        doluluk_df = summary.apply(hesapla_doluluk_satiri, axis=1)
-        summary = pd.concat([summary, doluluk_df], axis=1)
-        def renk_kodla(deger):
-            if deger &gt;= 95:
-                return 'background-color: lightgreen'
-            elif deger &gt;= 70:
-                return 'background-color: yellow'
-            else:
-                return 'background-color: lightcoral'
-        st.subheader("📊Araç Bazlı Özet")
-        styled_summary = summary.style \
-            .applymap(renk_kodla, subset=['DolulukOrani_Pallet']) \
-            .format({
-                'DolulukOrani_Pallet': "{:.1f}%",
-                'DolulukOrani_Volume': "{:.1f}%",
-                'DolulukOrani_Weight': "{:.1f}%"
-            })
-        st.dataframe(styled_summary, use_container_width=True, height=500)
-        # Yeni detaylı özet tablo (Araç + Ship-to bazlı)
-        truck_shipto_summary = assigned_df.groupby(
-            ['Assigned_Truck', 'Ship to', 'Ship to name', 'City_District','Sales Document','Requested delivery d']
-        )['EffectivePallet'].sum().reset_index()
-        st.subheader("Araç &amp; Ship-to Detaylı Özet")
-        st.dataframe(truck_shipto_summary, use_container_width=True, height=400)
-        # Excel çıktısı
-        output = BytesIO()
-        with pd.ExcelWriter(output, engine='xlsxwriter') as writer:
-            assigned_df.to_excel(writer, index=False, sheet_name='Atama Sonuçları')
-            summary.to_excel(writer, index=False, sheet_name='Araç Özeti')
-            truck_shipto_summary.to_excel(writer, index=False, sheet_name='Araç-ShipTo Özeti')
-        output.seek(0)
-        st.download_button(
-            label="📥 Excel İndir (Atama + Özetler)",
-            data=output,
-            file_name="order_arac_atama.xlsx",
-            mime="application/vnd.openxmlformats-officedocument.spreadsheetml.sheet"
-        )
-        </t>
-  </si>
-  <si>
     <t xml:space="preserve">import pandas as pd
 def palet_factor(pal_type):
     return 0.5 if pal_type == 'Kısa Hafif' else 1
@@ -522,6 +396,845 @@
     return assigned_df
 </t>
   </si>
+  <si>
+    <t>import streamlit as st
+import pandas as pd
+from solver import solve_assignment
+from io import BytesIO
+from PIL import Image
+# CSS ile yazı tipi ve boyutu ayarlayalım
+st.markdown("""
+    &lt;style&gt;
+        div[data-testid="stDataFrame"] div[role="gridcell"] {
+            font-family: Calibri, sans-serif;
+            font-size: 9pt;
+        }
+        .dataframe {
+            font-family: Calibri, sans-serif;
+            font-size: 9pt;
+        }
+    &lt;/style&gt;
+""", unsafe_allow_html=True)
+# Sayfanın başına ortalanmış resim ekle
+image = Image.open("Picture1.png")
+st.markdown("&lt;div style='text-align: center;'&gt;", unsafe_allow_html=True)
+st.image(image, width=300)
+st.markdown("&lt;/div&gt;", unsafe_allow_html=True)
+st.title("🚛 Load Planner")
+uploaded_file = st.file_uploader("Sipariş dosyasını yükleyin (Excel)", type=["xlsx"])
+if uploaded_file:
+    order_df = pd.read_excel(uploaded_file)
+    st.subheader("📝Yüklenen Sipariş Verisi")
+    st.dataframe(order_df, use_container_width=True, height=400)
+        # Bilgi Kartları Bölümü - Dosya yüklenince hemen çalışır
+    st.subheader("🔍 Veri Kalite Kontrolleri")
+    # 🛑 Sipariş Bazlı Palet Uyarısı
+    if 'EffectivePallet' in order_df.columns:
+        sales_pallet_summary = order_df.groupby("Sales Document")["EffectivePallet"].sum().reset_index()
+        over_limit_orders = sales_pallet_summary[sales_pallet_summary["EffectivePallet"] &gt; 33]
+        if not over_limit_orders.empty:
+            st.markdown("&lt;h4 style='color: red;'&gt;⚠️ Aşağıdaki siparişlerde toplam palet sayısı 33'ü geçiyor:&lt;/h4&gt;", unsafe_allow_html=True)
+            st.dataframe(over_limit_orders, use_container_width=True, height=250)
+    total_orders = order_df['Sales Document'].nunique()
+    missing_paltype = order_df[order_df['PALTypeChoice'].isna()]
+    missing_city = order_df[order_df['City_District'].isna()]
+    # Renk belirleme
+    paltype_color = "#90ee90" if missing_paltype.empty else "#ff7f7f"
+    city_color = "#90ee90" if missing_city.empty else "#ff7f7f"
+    col1, col2, col3 = st.columns(3)
+    with col1:
+        st.markdown(f"""
+            &lt;div style='padding: 20px; background-color: #90ee90; border-radius: 10px; text-align: center'&gt;
+                &lt;h4 style='margin: 0'&gt;Planda {total_orders} sipariş var&lt;/h4&gt;
+            &lt;/div&gt;
+        """, unsafe_allow_html=True)
+    with col2:
+        st.markdown(f"""
+            &lt;div style='padding: 20px; background-color: {paltype_color}; border-radius: 10px; text-align: center'&gt;
+                &lt;h4 style='margin: 0'&gt;
+                    {len(missing_paltype)} adet siparişin 'PALTypeChoice' bilgisi eksik.&lt;br&gt;Kontrol edin.
+                &lt;/h4&gt;
+            &lt;/div&gt;
+        """, unsafe_allow_html=True)
+    with col3:
+        st.markdown(f"""
+            &lt;div style='padding: 20px; background-color: {city_color}; border-radius: 10px; text-align: center'&gt;
+                &lt;h4 style='margin: 0'&gt;
+                    {missing_city['Ship to'].nunique()} adet müşterinin 'City_District' bilgisi eksik.&lt;br&gt;Kontrol edin.
+                &lt;/h4&gt;
+            &lt;/div&gt;
+        """, unsafe_allow_html=True)
+    if st.button("Araca Atamaları Yap"):
+        assigned_df = solve_assignment(order_df)
+        st.subheader("🚚 Atama Sonuçları")
+        st.dataframe(assigned_df, use_container_width=True, height=500)
+        # Araç bazlı özet tablo
+        summary = assigned_df.groupby("Assigned_Truck").agg({
+            'CPallet': 'sum',
+            'CPallet_M3': 'sum',
+            'CPallet_Gross': 'sum',
+            'EffectivePallet': 'sum'
+        }).reset_index()
+        # Doluluk hesaplaması: kamyon mu tır mı kontrol et
+        def hesapla_doluluk_satiri(row):
+            if row['EffectivePallet'] &lt;= 18:
+                palet_kapasite = 18
+                hacim_kapasite = 44
+                agirlik_kapasite = 12000
+            else:
+                palet_kapasite = 33
+                hacim_kapasite = 82
+                agirlik_kapasite = 24000
+            return pd.Series({
+                'DolulukOrani_Pallet': (row['EffectivePallet'] / palet_kapasite) * 100,
+                'DolulukOrani_Volume': (row['CPallet_M3'] / hacim_kapasite) * 100,
+                'DolulukOrani_Weight': (row['CPallet_Gross'] / agirlik_kapasite) * 100
+            })
+        doluluk_df = summary.apply(hesapla_doluluk_satiri, axis=1)
+        summary = pd.concat([summary, doluluk_df], axis=1)
+        def renk_kodla(deger):
+            if deger &gt;= 95:
+                return 'background-color: lightgreen'
+            elif deger &gt;= 70:
+                return 'background-color: yellow'
+            else:
+                return 'background-color: lightcoral'
+        st.subheader("📊Araç Bazlı Özet")
+        styled_summary = summary.style \
+            .applymap(renk_kodla, subset=['DolulukOrani_Pallet']) \
+            .format({
+                'DolulukOrani_Pallet': "{:.1f}%",
+                'DolulukOrani_Volume': "{:.1f}%",
+                'DolulukOrani_Weight': "{:.1f}%"
+            })
+        st.dataframe(styled_summary, use_container_width=True, height=500)
+        # Yeni detaylı özet tablo (Araç + Ship-to bazlı)
+        truck_shipto_summary = assigned_df.groupby(
+            ['Assigned_Truck', 'Ship to', 'Ship to name', 'City_District','Sales Document','Requested delivery d']
+        )['EffectivePallet'].sum().reset_index()
+        st.subheader("Araç &amp; Ship-to Detaylı Özet")
+        st.dataframe(truck_shipto_summary, use_container_width=True, height=400)
+        # Excel çıktısı
+        output = BytesIO()
+        with pd.ExcelWriter(output, engine='xlsxwriter') as writer:
+            assigned_df.to_excel(writer, index=False, sheet_name='Atama Sonuçları')
+            summary.to_excel(writer, index=False, sheet_name='Araç Özeti')
+            truck_shipto_summary.to_excel(writer, index=False, sheet_name='Araç-ShipTo Özeti')
+        output.seek(0)
+        st.download_button(
+            label="📥 Excel İndir (Atama + Özetler)",
+            data=output,
+            file_name="order_arac_atama.xlsx",
+            mime="application/vnd.openxmlformats-officedocument.spreadsheetml.sheet"
+        )
+        # 🛑 Sipariş Bazlı Palet Uyarısı
+        if 'EffectivePallet' in assigned_df.columns:
+            sales_pallet_summary = assigned_df.groupby("Sales Document")["EffectivePallet"].sum().reset_index()
+            over_limit_orders = sales_pallet_summary[sales_pallet_summary["EffectivePallet"] &gt; 33]
+            if not over_limit_orders.empty:
+                st.markdown("&lt;h4 style='color: red;'&gt;⚠️ Aşağıdaki siparişlerde toplam palet sayısı 33'ü geçiyor:&lt;/h4&gt;", unsafe_allow_html=True)
+                st.dataframe(over_limit_orders, use_container_width=True, height=250)</t>
+  </si>
+  <si>
+    <t>import streamlit as st
+import pandas as pd
+from solver import solve_assignment
+from io import BytesIO
+from PIL import Image
+import tempfile
+import os
+# COM Excel için
+try:
+    import win32com.client as win32
+except ImportError:
+    win32 = None  # yoksa pivot otomasyonu devre dışı kalacak
+# CSS ile yazı tipi ve boyutu ayarlayalım
+st.markdown("""
+    &lt;style&gt;
+        div[data-testid="stDataFrame"] div[role="gridcell"] {
+            font-family: Calibri, sans-serif;
+            font-size: 9pt;
+        }
+        .dataframe {
+            font-family: Calibri, sans-serif;
+            font-size: 9pt;
+        }
+    &lt;/style&gt;
+""", unsafe_allow_html=True)
+# Excel pivot table oluşturan fonksiyon (COM üzerinden, Windows + Excel gerekir)
+def create_excel_with_pivot_via_com(temp_path: str, output_path: str):
+    if win32 is None:
+        raise RuntimeError("win32com.client yüklü değil; gerçek pivot table oluşturulamaz.")
+    # Excel sabitlerinin sayısal karşılıkları
+    XL_DATABASE = 1          # xlDatabase
+    XL_ROW_FIELD = 1         # xlRowField
+    XL_SUM = -4157           # xlSum
+    excel = win32.DispatchEx("Excel.Application")
+    excel.Visible = False
+    excel.DisplayAlerts = False
+    try:
+        wb = excel.Workbooks.Open(temp_path)
+        # Veri sayfası
+        try:
+            data_ws = wb.Worksheets("Atama Sonuçları")
+        except Exception:
+            raise RuntimeError("Excel dosyasında 'Atama Sonuçları' sayfası yok.")
+        # Varsa eski pivot sayfasını sil
+        try:
+            existing = wb.Worksheets("Pivot Atama Sonuçları")
+            existing.Delete()
+        except Exception:
+            pass
+        pivot_ws = wb.Worksheets.Add()
+        pivot_ws.Name = "Pivot Atama Sonuçları"
+        # Veri aralığını al (A1'den başlayıp bitişiğe kadar)
+        source_range = data_ws.Range("A1").CurrentRegion
+        # Pivot cache oluştur
+        pivot_cache = wb.PivotCaches().Create(SourceType=XL_DATABASE, SourceData=source_range)
+        dest = pivot_ws.Range("A3")
+        pivot_table = pivot_cache.CreatePivotTable(TableDestination=dest, TableName="PivotTable1")
+        # Satır alanları: varsa ekle
+        for field in ["Assigned_Truck", "Ship to", "Sales Document","Ship to City", "Ship to name", "City_District"]:
+            try:
+                pf = pivot_table.PivotFields(field)
+                pf.Orientation = XL_ROW_FIELD
+            except Exception:
+                pass  # alan yoksa atla
+        # Değer alanı: EffectivePallet toplamı
+        try:
+            ep_field = pivot_table.PivotFields("EffectivePallet")
+            pivot_table.AddDataField(ep_field, "Sum of EffectivePallet", XL_SUM)
+        except Exception:
+            pass
+        pivot_table.RefreshTable()
+        wb.SaveAs(output_path)
+    finally:
+        wb.Close(SaveChanges=False)
+        excel.Quit()
+# Sayfanın başına ortalanmış resim ekle
+image = Image.open("Picture1.png")
+st.markdown("&lt;div style='text-align: center;'&gt;", unsafe_allow_html=True)
+st.image(image, width=300)
+st.markdown("&lt;/div&gt;", unsafe_allow_html=True)
+st.title("🚛 Load Planner")
+uploaded_file = st.file_uploader("Sipariş dosyasını yükleyin (Excel)", type=["xlsx"])
+if uploaded_file:
+    order_df = pd.read_excel(uploaded_file)
+    st.subheader("📝Yüklenen Sipariş Verisi")
+    st.dataframe(order_df, use_container_width=True, height=400)
+    # Bilgi Kartları Bölümü - Dosya kalite kontrolleri
+    st.subheader("🔍 Veri Kalite Kontrolleri")
+    if 'EffectivePallet' in order_df.columns:
+        sales_pallet_summary = order_df.groupby("Sales Document")["EffectivePallet"].sum().reset_index()
+        over_limit_orders = sales_pallet_summary[sales_pallet_summary["EffectivePallet"] &gt; 33]
+        if not over_limit_orders.empty:
+            st.markdown("&lt;h4 style='color: red;'&gt;⚠️ Aşağıdaki siparişlerde toplam palet sayısı 33'ü geçiyor:&lt;/h4&gt;", unsafe_allow_html=True)
+            st.dataframe(over_limit_orders, use_container_width=True, height=250)
+    total_orders = order_df['Sales Document'].nunique()
+    missing_paltype = order_df[order_df['PALTypeChoice'].isna()]
+    missing_city = order_df[order_df['City_District'].isna()]
+    paltype_color = "#90ee90" if missing_paltype.empty else "#ff7f7f"
+    city_color = "#90ee90" if missing_city.empty else "#ff7f7f"
+    col1, col2, col3 = st.columns(3)
+    with col1:
+        st.markdown(f"""
+            &lt;div style='padding: 20px; background-color: #90ee90; border-radius: 10px; text-align: center'&gt;
+                &lt;h4 style='margin: 0'&gt;Planda {total_orders} sipariş var&lt;/h4&gt;
+            &lt;/div&gt;
+        """, unsafe_allow_html=True)
+    with col2:
+        st.markdown(f"""
+            &lt;div style='padding: 20px; background-color: {paltype_color}; border-radius: 10px; text-align: center'&gt;
+                &lt;h4 style='margin: 0'&gt;
+                    {len(missing_paltype)} adet siparişin 'PALTypeChoice' bilgisi eksik.&lt;br&gt;Kontrol edin.
+                &lt;/h4&gt;
+            &lt;/div&gt;
+        """, unsafe_allow_html=True)
+    with col3:
+        st.markdown(f"""
+            &lt;div style='padding: 20px; background-color: {city_color}; border-radius: 10px; text-align: center'&gt;
+                &lt;h4 style='margin: 0'&gt;
+                    {missing_city['Ship to'].nunique()} adet müşterinin 'City_District' bilgisi eksik.&lt;br&gt;Kontrol edin.
+                &lt;/h4&gt;
+            &lt;/div&gt;
+        """, unsafe_allow_html=True)
+    if st.button("Araca Atamaları Yap"):
+        assigned_df = solve_assignment(order_df)
+        st.subheader("🚚 Atama Sonuçları")
+        st.dataframe(assigned_df, use_container_width=True, height=500)
+        # Araç bazlı özet tablo
+        summary = assigned_df.groupby("Assigned_Truck").agg({
+            'CPallet': 'sum',
+            'CPallet_M3': 'sum',
+            'CPallet_Gross': 'sum',
+            'EffectivePallet': 'sum'
+        }).reset_index()
+        # Doluluk hesaplaması
+        def hesapla_doluluk_satiri(row):
+            if row['EffectivePallet'] &lt;= 18:
+                palet_kapasite = 18
+                hacim_kapasite = 44
+                agirlik_kapasite = 12000
+            else:
+                palet_kapasite = 33
+                hacim_kapasite = 82
+                agirlik_kapasite = 24000
+            return pd.Series({
+                'DolulukOrani_Pallet': (row['EffectivePallet'] / palet_kapasite) * 100,
+                'DolulukOrani_Volume': (row['CPallet_M3'] / hacim_kapasite) * 100,
+                'DolulukOrani_Weight': (row['CPallet_Gross'] / agirlik_kapasite) * 100
+            })
+        doluluk_df = summary.apply(hesapla_doluluk_satiri, axis=1)
+        summary = pd.concat([summary, doluluk_df], axis=1)
+        def renk_kodla(deger):
+            if deger &gt;= 95:
+                return 'background-color: lightgreen'
+            elif deger &gt;= 70:
+                return 'background-color: yellow'
+            else:
+                return 'background-color: lightcoral'
+        st.subheader("📊Araç Bazlı Özet")
+        styled_summary = summary.style \
+            .applymap(renk_kodla, subset=['DolulukOrani_Pallet']) \
+            .format({
+                'DolulukOrani_Pallet': "{:.1f}%",
+                'DolulukOrani_Volume': "{:.1f}%",
+                'DolulukOrani_Weight': "{:.1f}%"
+            })
+        st.dataframe(styled_summary, use_container_width=True, height=500)
+        # Yeni detaylı özet tablo (Araç + Ship-to bazlı)
+        truck_shipto_summary = assigned_df.groupby(
+            ['Assigned_Truck', 'Ship to', 'Ship to name', 'City_District','Sales Document','Requested delivery d']
+        )['EffectivePallet'].sum().reset_index()
+        st.subheader("Araç &amp; Ship-to Detaylı Özet")
+        st.dataframe(truck_shipto_summary, use_container_width=True, height=400)
+        # Excel dosyasını önce geçiciye yaz
+        with tempfile.NamedTemporaryFile(suffix=".xlsx", delete=False) as tmp:
+            tmp_path = tmp.name
+        with pd.ExcelWriter(tmp_path, engine='xlsxwriter') as writer:
+            assigned_df.to_excel(writer, index=False, sheet_name='Atama Sonuçları')
+            summary.to_excel(writer, index=False, sheet_name='Araç Özeti')
+            truck_shipto_summary.to_excel(writer, index=False, sheet_name='Araç-ShipTo Özeti')
+        final_path = tmp_path.replace(".xlsx", "_pivot.xlsx")
+        try:
+            create_excel_with_pivot_via_com(tmp_path, final_path)
+            with open(final_path, "rb") as f:
+                data = f.read()
+            st.download_button(
+                label="📥 Excel İndir (Atama + Gerçek Pivot)",
+                data=data,
+                file_name="order_arac_atama_pivot.xlsx",
+                mime="application/vnd.openxmlformats-officedocument.spreadsheetml.sheet"
+            )
+        except Exception as e:
+            st.warning(f"Gerçek pivot oluşturulamadı: {e}. Excel dosyası pivot olmadan indiriliyor.")
+            with open(tmp_path, "rb") as f:
+                data = f.read()
+            st.download_button(
+                label="📥 Excel İndir (Atama + Özetler)",
+                data=data,
+                file_name="order_arac_atama.xlsx",
+                mime="application/vnd.openxmlformats-officedocument.spreadsheetml.sheet"
+            )
+        finally:
+            try:
+                os.remove(tmp_path)
+            except:
+                pass
+            try:
+                os.remove(final_path)
+            except:
+                pass
+        # 🛑 Sipariş Bazlı Palet Uyarısı
+        if 'EffectivePallet' in assigned_df.columns:
+            sales_pallet_summary = assigned_df.groupby("Sales Document")["EffectivePallet"].sum().reset_index()
+            over_limit_orders = sales_pallet_summary[sales_pallet_summary["EffectivePallet"] &gt; 33]
+            if not over_limit_orders.empty:
+                st.markdown("&lt;h4 style='color: red;'&gt;⚠️ Aşağıdaki siparişlerde toplam palet sayısı 33'ü geçiyor:&lt;/h4&gt;", unsafe_allow_html=True)
+                st.dataframe(over_limit_orders, use_container_width=True, height=250)</t>
+  </si>
+  <si>
+    <t>import pandas as pd
+def palet_factor(pal_type):
+    return 0.5 if pal_type == 'Kısa Hafif' else 1
+def calculate_effective_pallet(row):
+    return row['CPallet'] * palet_factor(row['PALTypeChoice'])
+def get_truck_limit(truck_type):
+    """Truck_Type sütununa göre araç palet limiti belirle"""
+    if pd.isna(truck_type):
+        return 33
+    t = truck_type.lower()
+    if "liftli" in t:
+        return 8
+    elif "kamyon" in t and "tır" not in t:
+        return 18
+    return 33  # Tır veya varsayılan
+def split_large_orders(city_group, truck_counter_start=1):
+    assignments = []
+    leftover_parts = []
+    truck_counter = truck_counter_start
+    shipto_groups = city_group.groupby('Ship to')
+    for ship_to, sub_group in shipto_groups:
+        truck_type = sub_group['Truck_Type'].iloc[0] if 'Truck_Type' in sub_group.columns else None
+        limit = get_truck_limit(truck_type)
+        total_pallet = sub_group['EffectivePallet'].sum()
+        if total_pallet &lt;= limit:
+            leftover_parts.append((ship_to, sub_group))
+            continue
+        rows = sub_group.to_dict('records')
+        part = []
+        part_load = 0
+        for row in rows:
+            p = row['EffectivePallet']
+            if part_load + p &gt; limit:
+                df_part = pd.DataFrame(part)
+                for r in df_part.to_dict('records'):
+                    r['Assigned_Truck'] = f"Truck-{truck_counter}"
+                    assignments.append(r)
+                truck_counter += 1
+                part = []
+                part_load = 0
+            part.append(row)
+            part_load += p
+        if part:
+            df_part = pd.DataFrame(part)
+            leftover_parts.append((ship_to, df_part))
+    return assignments, leftover_parts, truck_counter
+def group_and_assign_leftovers(leftover_parts, truck_counter_start=1):
+    assignments = []
+    truck_counter = truck_counter_start
+    combined_df = pd.concat([df for _, df in leftover_parts], ignore_index=True)
+    grouped_city = combined_df.groupby('Ship to City')
+    for city, city_group in grouped_city:
+        city_group = city_group.reset_index(drop=True)
+        subgroups = city_group.groupby('Ship to')
+        pending_groups = []
+        for ship_to, sub_group in subgroups:
+            total_pallet = sub_group['EffectivePallet'].sum()
+            pending_groups.append((ship_to, sub_group, total_pallet))
+        pending_groups.sort(key=lambda x: x[2], reverse=True)
+        while pending_groups:
+            current_load = 0
+            truck_orders = []
+            used_shiptos = set()
+            remaining_groups = []
+            def calc_adjusted_pallet(sub_group, multiple_shipto):
+                if not multiple_shipto:
+                    return sub_group['EffectivePallet'].sum()
+                else:
+                    def pallet_factor_override(row):
+                        return row['CPallet'] * 1  # KH'ler de KA gibi sayılır
+                    return sub_group.apply(pallet_factor_override, axis=1).sum()
+            for ship_to, sub_group, total_pallet in pending_groups:
+                multiple_shipto_in_truck = len(used_shiptos | {ship_to}) &gt; 1
+                adjusted_pallet = calc_adjusted_pallet(sub_group, multiple_shipto_in_truck)
+                truck_type = sub_group['Truck_Type'].iloc[0] if 'Truck_Type' in sub_group.columns else None
+                limit = get_truck_limit(truck_type)
+                if adjusted_pallet &lt;= limit:
+                    if (current_load + adjusted_pallet &lt;= limit) and (len(used_shiptos | {ship_to}) &lt;= 4):
+                        current_load += adjusted_pallet
+                        truck_orders.append((ship_to, sub_group))
+                        used_shiptos.add(ship_to)
+                    else:
+                        remaining_groups.append((ship_to, sub_group, total_pallet))
+                else:
+                    remaining_groups.append((ship_to, sub_group, total_pallet))
+            if truck_orders:
+                for ship_to, sub_group in truck_orders:
+                    for _, row in sub_group.iterrows():
+                        order = row.to_dict()
+                        order['Assigned_Truck'] = f"Truck-{truck_counter}"
+                        assignments.append(order)
+                truck_counter += 1
+            pending_groups = remaining_groups
+    return assignments, truck_counter
+def solve_assignment(order_df):
+    order_df = order_df.copy()
+    order_df.columns = order_df.columns.str.strip()
+    order_df = order_df.reset_index(drop=True)
+    if 'Ship to City' not in order_df.columns or 'Ship to' not in order_df.columns:
+        print("HATA: Gerekli sütunlar eksik!")
+        return pd.DataFrame()
+    try:
+        order_df['EffectivePallet'] = order_df.apply(calculate_effective_pallet, axis=1)
+    except Exception as e:
+        print("EffectivePallet hesaplamasında hata:", e)
+        return pd.DataFrame()
+    assignments = []
+    truck_counter = 1
+    grouped_city = order_df.groupby('Ship to City')
+    for city, city_group in grouped_city:
+        assigned_large, leftover_parts, truck_counter = split_large_orders(city_group, truck_counter)
+        assignments.extend(assigned_large)
+        assigned_leftovers, truck_counter = group_and_assign_leftovers(leftover_parts, truck_counter)
+        assignments.extend(assigned_leftovers)
+    assigned_df = pd.DataFrame(assignments)
+    def update_truck_name(truck_id, df):
+        has_temp = df['Temp_Type'].astype(str).str.contains('Temp').any()
+        truck_type = "Frigo" if has_temp else "Tente"
+        total_pallet = df['EffectivePallet'].sum()
+        vehicle_type = "Kamyon" if total_pallet &lt;= 18 else "Tır"
+        return f"{truck_type} {vehicle_type} -{truck_id}"
+    assigned_df['Truck_Number'] = assigned_df['Assigned_Truck'].str.extract(r'(\d+)').astype(int)
+    truck_names = {}
+    for truck_num, group in assigned_df.groupby('Truck_Number'):
+        truck_names[truck_num] = update_truck_name(truck_num, group)
+    assigned_df['Assigned_Truck'] = assigned_df['Truck_Number'].map(truck_names)
+    assigned_df = assigned_df.drop(columns=['Truck_Number'])
+    print(f"\n✅ Toplam atanan kayıt: {len(assigned_df)}")
+    return assigned_df</t>
+  </si>
+  <si>
+    <t>import pandas as pd
+def palet_factor(pal_type):
+    return 0.5 if pal_type == 'Kısa Hafif' else 1
+def calculate_effective_pallet(row):
+    return row['CPallet'] * palet_factor(row['PALTypeChoice'])
+def get_truck_limit(truck_type):
+    """Truck_Type sütununa göre araç palet limiti belirle"""
+    if pd.isna(truck_type):
+        return 33
+    t = truck_type.lower()
+    if "liftli" in t:
+        return 8
+    elif "kamyon" in t and "tır" not in t:
+        return 18
+    return 33  # Tır veya varsayılan
+def split_large_orders(city_group, truck_counter_start=1):
+    assignments = []
+    leftover_parts = []
+    truck_counter = truck_counter_start
+    shipto_groups = city_group.groupby('Ship to')
+    for ship_to, sub_group in shipto_groups:
+        truck_type = sub_group['Truck_Type'].iloc[0] if 'Truck_Type' in sub_group.columns else None
+        limit = get_truck_limit(truck_type)
+        total_pallet = sub_group['EffectivePallet'].sum()
+        if total_pallet &lt;= limit:
+            # ShipTo toplamı limit altında ise leftover olarak bırak
+            leftover_parts.append((ship_to, sub_group))
+            continue
+        # ShipTo toplamı limit aşıyor, Sales Document bazlı grupla ve atama yap
+        sales_groups = list(sub_group.groupby('Sales Document', dropna=False))
+        # Sales Document bazında toplam paletleri hesapla
+        sales_docs = []
+        for sd, df in sales_groups:
+            total_sd_pallet = df['EffectivePallet'].sum()
+            sales_docs.append((sd, df, total_sd_pallet))
+        # Satış belgelerini büyükten küçüğe sırala (greedy yerleştirme için)
+        sales_docs.sort(key=lambda x: x[2], reverse=True)
+        current_truck_load = 0
+        current_truck_docs = []
+        def flush_current_truck():
+            nonlocal truck_counter, current_truck_docs, current_truck_load
+            if not current_truck_docs:
+                return
+            combined_df = pd.concat([df for _, df, _ in current_truck_docs], ignore_index=True)
+            for _, row in combined_df.iterrows():
+                order = row.to_dict()
+                order['Assigned_Truck'] = f"Truck-{truck_counter}"
+                assignments.append(order)
+            truck_counter += 1
+            current_truck_docs = []
+            current_truck_load = 0
+        for sd, df, sd_total in sales_docs:
+            if sd_total &gt; limit:
+                # Eğer tek bir Sales Document bile limitten büyükse, kendi kamyonuna ata
+                for _, row in df.iterrows():
+                    order = row.to_dict()
+                    order['Assigned_Truck'] = f"Truck-{truck_counter}"
+                    assignments.append(order)
+                truck_counter += 1
+                continue
+            if current_truck_load + sd_total &lt;= limit:
+                current_truck_docs.append((sd, df, sd_total))
+                current_truck_load += sd_total
+            else:
+                flush_current_truck()
+                current_truck_docs.append((sd, df, sd_total))
+                current_truck_load = sd_total
+        # Son kalanları da ata
+        flush_current_truck()
+    return assignments, leftover_parts, truck_counter
+def group_and_assign_leftovers(leftover_parts, truck_counter_start=1):
+    assignments = []
+    truck_counter = truck_counter_start
+    # leftover_parts boş olabilir, bunu kontrol et
+    if not leftover_parts:
+        return assignments, truck_counter
+    # leftover_parts içindeki dfs gerçekten DataFrame mi kontrol et
+    dfs = [df for _, df in leftover_parts if isinstance(df, pd.DataFrame)]
+    if not dfs:
+        return assignments, truck_counter
+    combined_df = pd.concat(dfs, ignore_index=True)
+    grouped_city = combined_df.groupby('Ship to City')
+    for city, city_group in grouped_city:
+        city_group = city_group.reset_index(drop=True)
+        subgroups = city_group.groupby('Ship to')
+        pending_groups = []
+        for ship_to, sub_group in subgroups:
+            total_pallet = sub_group['EffectivePallet'].sum()
+            pending_groups.append((ship_to, sub_group, total_pallet))
+        pending_groups.sort(key=lambda x: x[2], reverse=True)
+        while pending_groups:
+            current_load = 0
+            truck_orders = []
+            used_shiptos = set()
+            remaining_groups = []
+            def calc_adjusted_pallet(sub_group, multiple_shipto):
+                if not multiple_shipto:
+                    return sub_group['EffectivePallet'].sum()
+                else:
+                    def pallet_factor_override(row):
+                        return row['CPallet'] * 1  # KH'ler de KA gibi sayılır
+                    return sub_group.apply(pallet_factor_override, axis=1).sum()
+            for ship_to, sub_group, total_pallet in pending_groups:
+                multiple_shipto_in_truck = len(used_shiptos | {ship_to}) &gt; 1
+                adjusted_pallet = calc_adjusted_pallet(sub_group, multiple_shipto_in_truck)
+                truck_type = sub_group['Truck_Type'].iloc[0] if 'Truck_Type' in sub_group.columns else None
+                limit = get_truck_limit(truck_type)
+                if adjusted_pallet &lt;= limit:
+                    if (current_load + adjusted_pallet &lt;= limit) and (len(used_shiptos | {ship_to}) &lt;= 4):
+                        current_load += adjusted_pallet
+                        truck_orders.append((ship_to, sub_group))
+                        used_shiptos.add(ship_to)
+                    else:
+                        remaining_groups.append((ship_to, sub_group, total_pallet))
+                else:
+                    remaining_groups.append((ship_to, sub_group, total_pallet))
+            if truck_orders:
+                for ship_to, sub_group in truck_orders:
+                    for _, row in sub_group.iterrows():
+                        order = row.to_dict()
+                        order['Assigned_Truck'] = f"Truck-{truck_counter}"
+                        assignments.append(order)
+                truck_counter += 1
+            pending_groups = remaining_groups
+    return assignments, truck_counter
+def solve_assignment(order_df):
+    order_df = order_df.copy()
+    order_df.columns = order_df.columns.str.strip()
+    order_df = order_df.reset_index(drop=True)
+    if 'Ship to City' not in order_df.columns or 'Ship to' not in order_df.columns:
+        print("HATA: Gerekli sütunlar eksik!")
+        return pd.DataFrame()
+    try:
+        order_df['EffectivePallet'] = order_df.apply(calculate_effective_pallet, axis=1)
+    except Exception as e:
+        print("EffectivePallet hesaplamasında hata:", e)
+        return pd.DataFrame()
+    assignments = []
+    truck_counter = 1
+    grouped_city = order_df.groupby('Ship to City')
+    for city, city_group in grouped_city:
+        assigned_large, leftover_parts, truck_counter = split_large_orders(city_group, truck_counter)
+        assignments.extend(assigned_large)
+        assigned_leftovers, truck_counter = group_and_assign_leftovers(leftover_parts, truck_counter)
+        assignments.extend(assigned_leftovers)
+    assigned_df = pd.DataFrame(assignments)
+    def update_truck_name(truck_id, df):
+        has_temp = df['Temp_Type'].astype(str).str.contains('Temp').any()
+        truck_type = "Frigo" if has_temp else "Tente"
+        total_pallet = df['EffectivePallet'].sum()
+        vehicle_type = "Kamyon" if total_pallet &lt;= 18 else "Tır"
+        return f"{truck_type} {vehicle_type} -{truck_id}"
+    assigned_df['Truck_Number'] = assigned_df['Assigned_Truck'].str.extract(r'(\d+)').astype(int)
+    truck_names = {}
+    for truck_num, group in assigned_df.groupby('Truck_Number'):
+        truck_names[truck_num] = update_truck_name(truck_num, group)
+    assigned_df['Assigned_Truck'] = assigned_df['Truck_Number'].map(truck_names)
+    assigned_df = assigned_df.drop(columns=['Truck_Number'])
+    print(f"\n✅ Toplam atanan kayıt: {len(assigned_df)}")
+    return assigned_df</t>
+  </si>
+  <si>
+    <t>import pandas as pd
+def palet_factor(pal_type):
+    return 0.5 if pal_type == 'Kısa Hafif' else 1
+def calculate_effective_pallet(row):
+    return row['CPallet'] * palet_factor(row['PALTypeChoice'])
+def get_truck_limit(truck_type):
+    if pd.isna(truck_type):
+        return 33
+    t = truck_type.lower()
+    if "liftli" in t:
+        return 8
+    elif "kamyon" in t and "tır" not in t:
+        return 18
+    return 33
+def split_sales_document_rows(df, limit, truck_counter_start):
+    """33 paleti geçen satış belgesini satır bazında bölerek atama yapar.
+    Satırları büyükten küçüğe sıralar, kamyonu mümkün olduğunca dolu tutmaya çalışır."""
+    assignments = []
+    truck_counter = truck_counter_start
+    # Satırları EffectivePallet'e göre büyükten küçüğe sırala
+    rows = df.to_dict('records')
+    rows.sort(key=lambda x: x['EffectivePallet'], reverse=True)
+    current_part = []
+    current_load = 0
+    for row in rows:
+        p = row['EffectivePallet']
+        # Eğer satırı eklemek 33'ü aşarsa, önce mevcut kamyonu atayıp yenisine başla
+        if current_load + p &gt; limit:
+            # Öncelikle mevcut partı at
+            if current_part:
+                for r in current_part:
+                    r['Assigned_Truck'] = f"Truck-{truck_counter}"
+                    assignments.append(r)
+                truck_counter += 1
+                current_part = []
+                current_load = 0
+        # Satırı yeni partiye ekle
+        current_part.append(row)
+        current_load += p
+    # Son part varsa ata
+    if current_part:
+        for r in current_part:
+            r['Assigned_Truck'] = f"Truck-{truck_counter}"
+            assignments.append(r)
+        truck_counter += 1
+    return assignments, truck_counter
+def split_large_orders(city_group, truck_counter_start=1):
+    assignments = []
+    leftover_parts = []
+    truck_counter = truck_counter_start
+    shipto_groups = city_group.groupby('Ship to')
+    for ship_to, sub_group in shipto_groups:
+        truck_type = sub_group['Truck_Type'].iloc[0] if 'Truck_Type' in sub_group.columns else None
+        limit = get_truck_limit(truck_type)
+        total_pallet = sub_group['EffectivePallet'].sum()
+        if total_pallet &lt;= limit:
+            leftover_parts.append((ship_to, sub_group))
+            continue
+        sales_groups = list(sub_group.groupby('Sales Document', dropna=False))
+        sales_docs = []
+        for sd, df in sales_groups:
+            total_sd_pallet = df['EffectivePallet'].sum()
+            sales_docs.append((sd, df, total_sd_pallet))
+        sales_docs.sort(key=lambda x: x[2], reverse=True)
+        current_truck_load = 0
+        current_truck_docs = []
+        def flush_current_truck():
+            nonlocal truck_counter, current_truck_docs, current_truck_load
+            if not current_truck_docs:
+                return
+            combined_df = pd.concat([df for _, df, _ in current_truck_docs], ignore_index=True)
+            for _, row in combined_df.iterrows():
+                order = row.to_dict()
+                order['Assigned_Truck'] = f"Truck-{truck_counter}"
+                assignments.append(order)
+            truck_counter += 1
+            current_truck_docs = []
+            current_truck_load = 0
+        for sd, df, sd_total in sales_docs:
+            if sd_total &gt; limit:
+                # 33 paleti geçen sales document için satır bazında bölme uygula
+                part_assignments, truck_counter = split_sales_document_rows(df, limit, truck_counter)
+                assignments.extend(part_assignments)
+                continue
+            if current_truck_load + sd_total &lt;= limit:
+                current_truck_docs.append((sd, df, sd_total))
+                current_truck_load += sd_total
+            else:
+                flush_current_truck()
+                current_truck_docs.append((sd, df, sd_total))
+                current_truck_load = sd_total
+        flush_current_truck()
+    return assignments, leftover_parts, truck_counter
+def group_and_assign_leftovers(leftover_parts, truck_counter_start=1):
+    assignments = []
+    truck_counter = truck_counter_start
+    if not leftover_parts:
+        return assignments, truck_counter
+    dfs = [df for _, df in leftover_parts if isinstance(df, pd.DataFrame)]
+    if not dfs:
+        return assignments, truck_counter
+    combined_df = pd.concat(dfs, ignore_index=True)
+    grouped_city = combined_df.groupby('Ship to City')
+    for city, city_group in grouped_city:
+        city_group = city_group.reset_index(drop=True)
+        subgroups = city_group.groupby('Ship to')
+        pending_groups = []
+        for ship_to, sub_group in subgroups:
+            total_pallet = sub_group['EffectivePallet'].sum()
+            pending_groups.append((ship_to, sub_group, total_pallet))
+        pending_groups.sort(key=lambda x: x[2], reverse=True)
+        while pending_groups:
+            current_load = 0
+            truck_orders = []
+            used_shiptos = set()
+            remaining_groups = []
+            def calc_adjusted_pallet(sub_group, multiple_shipto):
+                if not multiple_shipto:
+                    return sub_group['EffectivePallet'].sum()
+                else:
+                    def pallet_factor_override(row):
+                        return row['CPallet'] * 1
+                    return sub_group.apply(pallet_factor_override, axis=1).sum()
+            for ship_to, sub_group, total_pallet in pending_groups:
+                multiple_shipto_in_truck = len(used_shiptos | {ship_to}) &gt; 1
+                adjusted_pallet = calc_adjusted_pallet(sub_group, multiple_shipto_in_truck)
+                truck_type = sub_group['Truck_Type'].iloc[0] if 'Truck_Type' in sub_group.columns else None
+                limit = get_truck_limit(truck_type)
+                if adjusted_pallet &lt;= limit:
+                    if (current_load + adjusted_pallet &lt;= limit) and (len(used_shiptos | {ship_to}) &lt;= 4):
+                        current_load += adjusted_pallet
+                        truck_orders.append((ship_to, sub_group))
+                        used_shiptos.add(ship_to)
+                    else:
+                        remaining_groups.append((ship_to, sub_group, total_pallet))
+                else:
+                    remaining_groups.append((ship_to, sub_group, total_pallet))
+            if truck_orders:
+                for ship_to, sub_group in truck_orders:
+                    for _, row in sub_group.iterrows():
+                        order = row.to_dict()
+                        order['Assigned_Truck'] = f"Truck-{truck_counter}"
+                        assignments.append(order)
+                truck_counter += 1
+            pending_groups = remaining_groups
+    return assignments, truck_counter
+def solve_assignment(order_df):
+    order_df = order_df.copy()
+    order_df.columns = order_df.columns.str.strip()
+    order_df = order_df.reset_index(drop=True)
+    if 'Ship to City' not in order_df.columns or 'Ship to' not in order_df.columns:
+        print("HATA: Gerekli sütunlar eksik!")
+        return pd.DataFrame()
+    try:
+        order_df['EffectivePallet'] = order_df.apply(calculate_effective_pallet, axis=1)
+    except Exception as e:
+        print("EffectivePallet hesaplamasında hata:", e)
+        return pd.DataFrame()
+    assignments = []
+    truck_counter = 1
+    grouped_city = order_df.groupby('Ship to City')
+    for city, city_group in grouped_city:
+        assigned_large, leftover_parts, truck_counter = split_large_orders(city_group, truck_counter)
+        assignments.extend(assigned_large)
+        assigned_leftovers, truck_counter = group_and_assign_leftovers(leftover_parts, truck_counter)
+        assignments.extend(assigned_leftovers)
+    assigned_df = pd.DataFrame(assignments)
+    def update_truck_name(truck_id, df):
+        has_temp = df['Temp_Type'].astype(str).str.contains('Temp').any()
+        truck_type = "Frigo" if has_temp else "Tente"
+        total_pallet = df['EffectivePallet'].sum()
+        vehicle_type = "Kamyon" if total_pallet &lt;= 18 else "Tır"
+        return f"{truck_type} {vehicle_type} -{truck_id}"
+    assigned_df['Truck_Number'] = assigned_df['Assigned_Truck'].str.extract(r'(\d+)').astype(int)
+    truck_names = {}
+    for truck_num, group in assigned_df.groupby('Truck_Number'):
+        truck_names[truck_num] = update_truck_name(truck_num, group)
+    assigned_df['Assigned_Truck'] = assigned_df['Truck_Number'].map(truck_names)
+    assigned_df = assigned_df.drop(columns=['Truck_Number'])
+    print(f"\n✅ Toplam atanan kayıt: {len(assigned_df)}")
+    return assigned_df</t>
+  </si>
+  <si>
+    <t>1.08.2025-33 bölmesiz</t>
+  </si>
+  <si>
+    <t>1.08.2025-33 palet bölmeli</t>
+  </si>
 </sst>
 </file>
 
@@ -597,7 +1310,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -612,6 +1325,14 @@
     <xf numFmtId="16" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -946,7 +1667,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC0E7DBC-2E6E-483B-B2B4-F781243CD46F}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
@@ -957,11 +1678,13 @@
     <col min="1" max="1" width="16.81640625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.453125" style="1" customWidth="1"/>
     <col min="3" max="3" width="16.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.453125" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="16.7265625" style="1"/>
+    <col min="4" max="5" width="17.453125" style="1" customWidth="1"/>
+    <col min="6" max="7" width="16.7265625" style="1"/>
+    <col min="8" max="8" width="16.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="16.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>4</v>
       </c>
@@ -974,8 +1697,20 @@
       <c r="D1" s="5">
         <v>45821</v>
       </c>
+      <c r="E1" s="6">
+        <v>45869</v>
+      </c>
+      <c r="F1" s="6">
+        <v>45869</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" ht="18.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="18.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -988,8 +1723,20 @@
       <c r="D2" s="2" t="s">
         <v>1</v>
       </c>
+      <c r="E2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -997,10 +1744,22 @@
         <v>3</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>5</v>
+      <c r="E3" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>